<commit_message>
Commit another version of the lipid data
</commit_message>
<xml_diff>
--- a/data/Lipid concentration_diel (from KB).xlsx
+++ b/data/Lipid concentration_diel (from KB).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34980" yWindow="460" windowWidth="30680" windowHeight="19840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="As received from KB" sheetId="1" r:id="rId1"/>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2362,7 +2362,7 @@
   <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D3" sqref="D3:O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>